<commit_message>
Update predictions with login column
</commit_message>
<xml_diff>
--- a/predictions.xlsx
+++ b/predictions.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="vijay" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,6 +454,11 @@
           <t>Match Winner</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Login</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -474,6 +479,34 @@
       <c r="D2" t="inlineStr">
         <is>
           <t>Kolkata Knight Riders</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>22-03-2025</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Kolkata Knight Riders vs Royal Challengers Bengaluru</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Kolkata Knight Riders</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Kolkata Knight Riders</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>vijay</t>
         </is>
       </c>
     </row>

</xml_diff>